<commit_message>
translation, last change fr
</commit_message>
<xml_diff>
--- a/data/poverty/WID_income.xlsx
+++ b/data/poverty/WID_income.xlsx
@@ -5,7 +5,7 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabre\Documents\www\global_tax_attitudes\data\poverty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabre\Documents\www\plan_mondial_climat\data\poverty\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="22" uniqueCount="21">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="26" uniqueCount="23">
   <si>
     <t>Downloaded from wid.world on 29-04-2024 at 12:05:28</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>monthly average</t>
+  </si>
+  <si>
+    <t>European Union</t>
+  </si>
+  <si>
+    <t>p97p100</t>
   </si>
 </sst>
 </file>
@@ -917,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,10 +1195,60 @@
         <v>9.4034999999999993</v>
       </c>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="3"/>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>2022</v>
+      </c>
+      <c r="C18" s="3">
+        <v>119588.4</v>
+      </c>
+      <c r="D18" s="3">
+        <f>C18/12</f>
+        <v>9965.6999999999989</v>
+      </c>
+      <c r="E18" s="3">
+        <v>240624.5</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" ref="F18:F19" si="2">E18/12</f>
+        <v>20052.041666666668</v>
+      </c>
+      <c r="G18" s="1">
+        <f>(100/3)*E19/(E18-C18)</f>
+        <v>8.1780008884401706E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3">
+        <v>296.95</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>24.745833333333334</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>